<commit_message>
Changing opacity of water back to 1 - this appears to be what vanilla Minecraft actually uses.
</commit_message>
<xml_diff>
--- a/Reference/Minecraft Block Values.xlsx
+++ b/Reference/Minecraft Block Values.xlsx
@@ -914,7 +914,7 @@
         <v>12</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -947,7 +947,7 @@
         <v>12</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>

</xml_diff>